<commit_message>
Вт 24.11.20 : 20:35:38,20
</commit_message>
<xml_diff>
--- a/eng.xlsx
+++ b/eng.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="124">
   <si>
     <t>Стек</t>
   </si>
@@ -224,9 +224,6 @@
   </si>
   <si>
     <t>Start</t>
-  </si>
-  <si>
-    <t>1F</t>
   </si>
   <si>
     <t>N (число) N01</t>
@@ -390,6 +387,12 @@
   </si>
   <si>
     <t>UPL</t>
+  </si>
+  <si>
+    <t>Push(2A),State(0)</t>
+  </si>
+  <si>
+    <t>F1</t>
   </si>
 </sst>
 </file>
@@ -574,7 +577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -687,6 +690,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2483,8 +2489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2510,13 +2516,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="42" t="s">
         <v>69</v>
-      </c>
-      <c r="C1" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>70</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>2</v>
@@ -2552,31 +2558,31 @@
         <v>31</v>
       </c>
       <c r="P1" s="42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q1" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="R1" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="S1" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="S1" s="34" t="s">
+      <c r="T1" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="T1" s="34" t="s">
+      <c r="U1" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="U1" s="34" t="s">
+      <c r="V1" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="V1" s="34" t="s">
+      <c r="W1" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="W1" s="34" t="s">
+      <c r="X1" s="34" t="s">
         <v>83</v>
-      </c>
-      <c r="X1" s="34" t="s">
-        <v>84</v>
       </c>
       <c r="Y1" s="43" t="s">
         <v>58</v>
@@ -2588,7 +2594,7 @@
         <v>4</v>
       </c>
       <c r="AB1" s="43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2596,16 +2602,16 @@
         <v>67</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>36</v>
@@ -2620,49 +2626,49 @@
         <v>40</v>
       </c>
       <c r="J2" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="K2" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" s="20" t="s">
+      <c r="N2" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="N2" s="20" t="s">
-        <v>99</v>
-      </c>
       <c r="O2" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P2" s="19" t="s">
         <v>36</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R2" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S2" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T2" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U2" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V2" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W2" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X2" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y2" s="19" t="s">
         <v>36</v>
@@ -2674,7 +2680,7 @@
         <v>36</v>
       </c>
       <c r="AB2" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2682,19 +2688,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G3" s="19" t="s">
         <v>36</v>
@@ -2730,25 +2736,25 @@
         <v>36</v>
       </c>
       <c r="R3" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S3" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T3" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U3" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V3" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W3" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X3" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y3" s="19" t="s">
         <v>36</v>
@@ -2765,28 +2771,28 @@
     </row>
     <row r="4" spans="1:28" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>91</v>
-      </c>
       <c r="H4" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I4" s="19" t="s">
         <v>36</v>
@@ -2816,25 +2822,25 @@
         <v>36</v>
       </c>
       <c r="R4" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S4" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T4" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U4" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V4" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W4" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X4" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y4" s="19" t="s">
         <v>36</v>
@@ -2851,28 +2857,28 @@
     </row>
     <row r="5" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>91</v>
-      </c>
       <c r="G5" s="19" t="s">
         <v>36</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I5" s="19" t="s">
         <v>36</v>
@@ -2902,25 +2908,25 @@
         <v>36</v>
       </c>
       <c r="R5" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S5" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T5" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U5" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V5" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W5" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X5" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y5" s="19" t="s">
         <v>36</v>
@@ -2940,16 +2946,16 @@
         <v>9</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>36</v>
@@ -2967,7 +2973,7 @@
         <v>36</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L6" s="19" t="s">
         <v>36</v>
@@ -2988,25 +2994,25 @@
         <v>36</v>
       </c>
       <c r="R6" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S6" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T6" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U6" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V6" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W6" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X6" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y6" s="19" t="s">
         <v>36</v>
@@ -3023,40 +3029,40 @@
     </row>
     <row r="7" spans="1:28" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E7" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="J7" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="F7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>97</v>
-      </c>
       <c r="K7" s="19" t="s">
         <v>36</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M7" s="19" t="s">
         <v>36</v>
@@ -3071,28 +3077,28 @@
         <v>36</v>
       </c>
       <c r="Q7" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R7" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S7" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T7" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U7" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V7" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W7" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X7" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y7" s="19" t="s">
         <v>36</v>
@@ -3109,40 +3115,40 @@
     </row>
     <row r="8" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E8" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="J8" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="J8" s="20" t="s">
-        <v>97</v>
-      </c>
       <c r="K8" s="19" t="s">
         <v>36</v>
       </c>
       <c r="L8" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M8" s="19" t="s">
         <v>36</v>
@@ -3157,28 +3163,28 @@
         <v>36</v>
       </c>
       <c r="Q8" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R8" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S8" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T8" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U8" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V8" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W8" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X8" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y8" s="19" t="s">
         <v>36</v>
@@ -3195,7 +3201,7 @@
     </row>
     <row r="9" spans="1:28" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>36</v>
@@ -3204,10 +3210,10 @@
         <v>36</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F9" s="19" t="s">
         <v>36</v>
@@ -3219,7 +3225,7 @@
         <v>36</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J9" s="19" t="s">
         <v>36</v>
@@ -3281,7 +3287,7 @@
     </row>
     <row r="10" spans="1:28" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>36</v>
@@ -3290,7 +3296,7 @@
         <v>36</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>40</v>
@@ -3302,10 +3308,10 @@
         <v>36</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J10" s="19" t="s">
         <v>36</v>
@@ -3326,7 +3332,7 @@
         <v>36</v>
       </c>
       <c r="P10" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q10" s="19" t="s">
         <v>36</v>
@@ -3367,31 +3373,31 @@
     </row>
     <row r="11" spans="1:28" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="23" t="s">
+      <c r="I11" s="23" t="s">
         <v>119</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>120</v>
       </c>
       <c r="J11" s="19" t="s">
         <v>36</v>
@@ -3477,7 +3483,7 @@
         <v>36</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J12" s="19" t="s">
         <v>36</v>
@@ -3525,7 +3531,7 @@
         <v>36</v>
       </c>
       <c r="Y12" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Z12" s="19" t="s">
         <v>36</v>
@@ -3539,19 +3545,19 @@
     </row>
     <row r="13" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>36</v>
@@ -3563,7 +3569,7 @@
         <v>36</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J13" s="19" t="s">
         <v>36</v>
@@ -3572,7 +3578,7 @@
         <v>36</v>
       </c>
       <c r="L13" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M13" s="19" t="s">
         <v>36</v>
@@ -3590,25 +3596,25 @@
         <v>36</v>
       </c>
       <c r="R13" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S13" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T13" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U13" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V13" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W13" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X13" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y13" s="19" t="s">
         <v>36</v>
@@ -3625,31 +3631,31 @@
     </row>
     <row r="14" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I14" s="45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J14" s="19" t="s">
         <v>36</v>
@@ -3676,25 +3682,25 @@
         <v>36</v>
       </c>
       <c r="R14" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S14" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T14" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U14" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V14" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W14" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X14" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y14" s="19" t="s">
         <v>36</v>
@@ -3711,31 +3717,31 @@
     </row>
     <row r="15" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I15" s="45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J15" s="19" t="s">
         <v>36</v>
@@ -3762,25 +3768,25 @@
         <v>36</v>
       </c>
       <c r="R15" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S15" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T15" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U15" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V15" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W15" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X15" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y15" s="19" t="s">
         <v>36</v>
@@ -3797,31 +3803,31 @@
     </row>
     <row r="16" spans="1:28" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J16" s="19" t="s">
         <v>36</v>
@@ -3848,25 +3854,25 @@
         <v>36</v>
       </c>
       <c r="R16" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S16" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T16" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="U16" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V16" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W16" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X16" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y16" s="19" t="s">
         <v>36</v>
@@ -3883,31 +3889,31 @@
     </row>
     <row r="17" spans="1:28" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J17" s="19" t="s">
         <v>36</v>
@@ -3934,25 +3940,25 @@
         <v>36</v>
       </c>
       <c r="R17" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S17" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T17" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="U17" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="V17" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W17" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X17" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y17" s="19" t="s">
         <v>36</v>
@@ -3969,31 +3975,31 @@
     </row>
     <row r="18" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H18" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J18" s="19" t="s">
         <v>36</v>
@@ -4020,25 +4026,25 @@
         <v>36</v>
       </c>
       <c r="R18" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S18" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T18" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="U18" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="V18" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="W18" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X18" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y18" s="19" t="s">
         <v>36</v>
@@ -4055,31 +4061,31 @@
     </row>
     <row r="19" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H19" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J19" s="19" t="s">
         <v>36</v>
@@ -4106,25 +4112,25 @@
         <v>36</v>
       </c>
       <c r="R19" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S19" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T19" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="U19" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="V19" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="W19" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="X19" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>36</v>
@@ -4141,31 +4147,31 @@
     </row>
     <row r="20" spans="1:28" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J20" s="19" t="s">
         <v>36</v>
@@ -4192,25 +4198,25 @@
         <v>36</v>
       </c>
       <c r="R20" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S20" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T20" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="U20" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="V20" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="W20" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="X20" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Y20" s="19" t="s">
         <v>36</v>
@@ -4227,10 +4233,10 @@
     </row>
     <row r="21" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="20" t="s">
         <v>113</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>114</v>
       </c>
       <c r="C21" s="19" t="s">
         <v>36</v>
@@ -4313,10 +4319,10 @@
     </row>
     <row r="22" spans="1:28" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C22" s="19" t="s">
         <v>36</v>
@@ -4397,7 +4403,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:28" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="31"/>
+    </row>
     <row r="24" spans="1:28" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="35" t="s">
         <v>0</v>
@@ -4408,27 +4416,33 @@
       <c r="C24" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="E24" s="27" t="s">
+      <c r="D24" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24" s="27" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="36" t="s">
-        <v>68</v>
+        <v>123</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="D25" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="E25" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" s="30" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4437,34 +4451,37 @@
         <v>64</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26" s="33" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="33" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B27" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:28" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B30" s="20" t="s">
         <v>65</v>
@@ -4472,18 +4489,18 @@
     </row>
     <row r="31" spans="1:28" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:28" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Вт 24.11.20 : 20:50:36,53
</commit_message>
<xml_diff>
--- a/eng.xlsx
+++ b/eng.xlsx
@@ -2489,8 +2489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Вт 24.11.20 : 21:45:40,13
</commit_message>
<xml_diff>
--- a/eng.xlsx
+++ b/eng.xlsx
@@ -2489,8 +2489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Ср 25.11.20 :  9:58:52,80
</commit_message>
<xml_diff>
--- a/eng.xlsx
+++ b/eng.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="126">
   <si>
     <t>Стек</t>
   </si>
@@ -238,9 +238,6 @@
     <t>Fi</t>
   </si>
   <si>
-    <t xml:space="preserve">Proc_i,j </t>
-  </si>
-  <si>
     <t xml:space="preserve">IF_mi+1 </t>
   </si>
   <si>
@@ -313,12 +310,6 @@
     <t>Push(IF)</t>
   </si>
   <si>
-    <t>Push(i,j_Proc)</t>
-  </si>
-  <si>
-    <t>Push(i,j_D)</t>
-  </si>
-  <si>
     <t>Push(1F)</t>
   </si>
   <si>
@@ -344,9 +335,6 @@
   </si>
   <si>
     <t>Swap(i+1_F)</t>
-  </si>
-  <si>
-    <t>Swap(i,j,k+1_D)</t>
   </si>
   <si>
     <t>Pop(X),Swap(2F),State(0)</t>
@@ -377,9 +365,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>Pop(k_type),getOut,Swap(i,j,k+1_D)</t>
-  </si>
-  <si>
     <t>Pop(k_type),getOut,Hold</t>
   </si>
   <si>
@@ -393,6 +378,27 @@
   </si>
   <si>
     <t>F1</t>
+  </si>
+  <si>
+    <t>Pop(:),State(0)</t>
+  </si>
+  <si>
+    <t>begin</t>
+  </si>
+  <si>
+    <t>Push(i_j_D)</t>
+  </si>
+  <si>
+    <t>Swap(i_j_k+1_D)</t>
+  </si>
+  <si>
+    <t>Pop(k_type),getOut,Swap(i_j_k+1_D)</t>
+  </si>
+  <si>
+    <t>Pop(i_j_NP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proc_i,j </t>
   </si>
 </sst>
 </file>
@@ -2489,8 +2495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2519,7 +2525,7 @@
         <v>68</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D1" s="42" t="s">
         <v>69</v>
@@ -2549,7 +2555,7 @@
         <v>28</v>
       </c>
       <c r="M1" s="42" t="s">
-        <v>29</v>
+        <v>120</v>
       </c>
       <c r="N1" s="42" t="s">
         <v>61</v>
@@ -2558,31 +2564,31 @@
         <v>31</v>
       </c>
       <c r="P1" s="42" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="Q1" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="R1" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="S1" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="S1" s="34" t="s">
+      <c r="T1" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="T1" s="34" t="s">
+      <c r="U1" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="U1" s="34" t="s">
+      <c r="V1" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="V1" s="34" t="s">
+      <c r="W1" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="W1" s="34" t="s">
+      <c r="X1" s="34" t="s">
         <v>82</v>
-      </c>
-      <c r="X1" s="34" t="s">
-        <v>83</v>
       </c>
       <c r="Y1" s="43" t="s">
         <v>58</v>
@@ -2594,7 +2600,7 @@
         <v>4</v>
       </c>
       <c r="AB1" s="43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2602,16 +2608,16 @@
         <v>67</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>36</v>
@@ -2626,7 +2632,7 @@
         <v>40</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K2" s="19" t="s">
         <v>36</v>
@@ -2635,40 +2641,40 @@
         <v>36</v>
       </c>
       <c r="M2" s="20" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P2" s="19" t="s">
         <v>36</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R2" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S2" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T2" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U2" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="V2" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W2" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X2" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Y2" s="19" t="s">
         <v>36</v>
@@ -2680,7 +2686,7 @@
         <v>36</v>
       </c>
       <c r="AB2" s="18" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2688,19 +2694,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G3" s="19" t="s">
         <v>36</v>
@@ -2736,25 +2742,25 @@
         <v>36</v>
       </c>
       <c r="R3" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S3" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T3" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U3" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="V3" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W3" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X3" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Y3" s="19" t="s">
         <v>36</v>
@@ -2774,25 +2780,25 @@
         <v>70</v>
       </c>
       <c r="B4" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>90</v>
-      </c>
       <c r="H4" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I4" s="19" t="s">
         <v>36</v>
@@ -2822,25 +2828,25 @@
         <v>36</v>
       </c>
       <c r="R4" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S4" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T4" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U4" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="V4" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W4" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X4" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Y4" s="19" t="s">
         <v>36</v>
@@ -2860,25 +2866,25 @@
         <v>71</v>
       </c>
       <c r="B5" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>90</v>
-      </c>
       <c r="G5" s="19" t="s">
         <v>36</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I5" s="19" t="s">
         <v>36</v>
@@ -2908,25 +2914,25 @@
         <v>36</v>
       </c>
       <c r="R5" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S5" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T5" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U5" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="V5" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W5" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X5" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Y5" s="19" t="s">
         <v>36</v>
@@ -2946,16 +2952,16 @@
         <v>9</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>36</v>
@@ -2973,7 +2979,7 @@
         <v>36</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L6" s="19" t="s">
         <v>36</v>
@@ -2994,25 +3000,25 @@
         <v>36</v>
       </c>
       <c r="R6" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S6" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T6" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U6" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="V6" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W6" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X6" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Y6" s="19" t="s">
         <v>36</v>
@@ -3029,40 +3035,40 @@
     </row>
     <row r="7" spans="1:28" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E7" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="F7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>96</v>
-      </c>
       <c r="K7" s="19" t="s">
         <v>36</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="M7" s="19" t="s">
         <v>36</v>
@@ -3077,28 +3083,28 @@
         <v>36</v>
       </c>
       <c r="Q7" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R7" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S7" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T7" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U7" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="V7" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W7" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X7" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Y7" s="19" t="s">
         <v>36</v>
@@ -3115,40 +3121,40 @@
     </row>
     <row r="8" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E8" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="J8" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="F8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="J8" s="20" t="s">
-        <v>96</v>
-      </c>
       <c r="K8" s="19" t="s">
         <v>36</v>
       </c>
       <c r="L8" s="20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="M8" s="19" t="s">
         <v>36</v>
@@ -3163,28 +3169,28 @@
         <v>36</v>
       </c>
       <c r="Q8" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R8" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S8" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T8" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U8" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="V8" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W8" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X8" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Y8" s="19" t="s">
         <v>36</v>
@@ -3201,7 +3207,7 @@
     </row>
     <row r="9" spans="1:28" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
-        <v>72</v>
+        <v>125</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>36</v>
@@ -3210,10 +3216,10 @@
         <v>36</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F9" s="19" t="s">
         <v>36</v>
@@ -3225,7 +3231,7 @@
         <v>36</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J9" s="19" t="s">
         <v>36</v>
@@ -3287,7 +3293,7 @@
     </row>
     <row r="10" spans="1:28" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>36</v>
@@ -3296,7 +3302,7 @@
         <v>36</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>40</v>
@@ -3308,10 +3314,10 @@
         <v>36</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J10" s="19" t="s">
         <v>36</v>
@@ -3332,7 +3338,7 @@
         <v>36</v>
       </c>
       <c r="P10" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q10" s="19" t="s">
         <v>36</v>
@@ -3373,7 +3379,7 @@
     </row>
     <row r="11" spans="1:28" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>36</v>
@@ -3394,10 +3400,10 @@
         <v>36</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="J11" s="19" t="s">
         <v>36</v>
@@ -3483,7 +3489,7 @@
         <v>36</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="J12" s="19" t="s">
         <v>36</v>
@@ -3531,7 +3537,7 @@
         <v>36</v>
       </c>
       <c r="Y12" s="16" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Z12" s="19" t="s">
         <v>36</v>
@@ -3545,19 +3551,19 @@
     </row>
     <row r="13" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>36</v>
@@ -3569,7 +3575,7 @@
         <v>36</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J13" s="19" t="s">
         <v>36</v>
@@ -3578,7 +3584,7 @@
         <v>36</v>
       </c>
       <c r="L13" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="M13" s="19" t="s">
         <v>36</v>
@@ -3596,25 +3602,25 @@
         <v>36</v>
       </c>
       <c r="R13" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S13" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T13" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U13" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="V13" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W13" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X13" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Y13" s="19" t="s">
         <v>36</v>
@@ -3631,31 +3637,31 @@
     </row>
     <row r="14" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I14" s="45" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J14" s="19" t="s">
         <v>36</v>
@@ -3682,25 +3688,25 @@
         <v>36</v>
       </c>
       <c r="R14" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="S14" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T14" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U14" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="V14" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W14" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X14" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Y14" s="19" t="s">
         <v>36</v>
@@ -3717,31 +3723,31 @@
     </row>
     <row r="15" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I15" s="45" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J15" s="19" t="s">
         <v>36</v>
@@ -3768,25 +3774,25 @@
         <v>36</v>
       </c>
       <c r="R15" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="S15" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="T15" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U15" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="V15" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W15" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X15" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Y15" s="19" t="s">
         <v>36</v>
@@ -3803,31 +3809,31 @@
     </row>
     <row r="16" spans="1:28" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J16" s="19" t="s">
         <v>36</v>
@@ -3854,25 +3860,25 @@
         <v>36</v>
       </c>
       <c r="R16" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="S16" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="T16" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="U16" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="V16" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W16" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X16" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Y16" s="19" t="s">
         <v>36</v>
@@ -3889,31 +3895,31 @@
     </row>
     <row r="17" spans="1:28" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J17" s="19" t="s">
         <v>36</v>
@@ -3940,25 +3946,25 @@
         <v>36</v>
       </c>
       <c r="R17" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="S17" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="T17" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="U17" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="V17" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W17" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X17" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Y17" s="19" t="s">
         <v>36</v>
@@ -3975,31 +3981,31 @@
     </row>
     <row r="18" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H18" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J18" s="19" t="s">
         <v>36</v>
@@ -4026,25 +4032,25 @@
         <v>36</v>
       </c>
       <c r="R18" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="S18" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="T18" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="U18" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="V18" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="W18" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X18" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Y18" s="19" t="s">
         <v>36</v>
@@ -4061,31 +4067,31 @@
     </row>
     <row r="19" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H19" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J19" s="19" t="s">
         <v>36</v>
@@ -4112,25 +4118,25 @@
         <v>36</v>
       </c>
       <c r="R19" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="S19" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="T19" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="U19" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="V19" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="W19" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="X19" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>36</v>
@@ -4147,31 +4153,31 @@
     </row>
     <row r="20" spans="1:28" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J20" s="19" t="s">
         <v>36</v>
@@ -4198,25 +4204,25 @@
         <v>36</v>
       </c>
       <c r="R20" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="S20" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="T20" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="U20" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="V20" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="W20" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="X20" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="Y20" s="19" t="s">
         <v>36</v>
@@ -4233,10 +4239,10 @@
     </row>
     <row r="21" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C21" s="19" t="s">
         <v>36</v>
@@ -4319,10 +4325,10 @@
     </row>
     <row r="22" spans="1:28" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C22" s="19" t="s">
         <v>36</v>
@@ -4420,29 +4426,35 @@
         <v>4</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="F24" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="27" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="36" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C25" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="D25" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>109</v>
-      </c>
       <c r="F25" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="30" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4451,37 +4463,40 @@
         <v>64</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E26" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="33" t="s">
-        <v>105</v>
+      <c r="F26" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="G26" s="33" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B27" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:28" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="39" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B30" s="20" t="s">
         <v>65</v>
@@ -4489,18 +4504,18 @@
     </row>
     <row r="31" spans="1:28" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:28" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ср 25.11.20 : 10:41:25,74
</commit_message>
<xml_diff>
--- a/eng.xlsx
+++ b/eng.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="128">
   <si>
     <t>Стек</t>
   </si>
@@ -338,9 +338,6 @@
   </si>
   <si>
     <t>Pop(X),Swap(2F),State(0)</t>
-  </si>
-  <si>
-    <t>Push(BP)</t>
   </si>
   <si>
     <t>Pop(Mi+1_BP_Mi:), Swap(Mi+1_IF)</t>
@@ -399,6 +396,15 @@
   </si>
   <si>
     <t xml:space="preserve">proc_i,j </t>
+  </si>
+  <si>
+    <t>Push(GOTO)</t>
+  </si>
+  <si>
+    <t>Метка</t>
+  </si>
+  <si>
+    <t>Swap(G),Pop,getOut,Pop(BP)</t>
   </si>
 </sst>
 </file>
@@ -2493,10 +2499,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB33"/>
+  <dimension ref="A1:AC34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2517,7 +2523,7 @@
     <col min="28" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="43" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" s="43" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
@@ -2525,7 +2531,7 @@
         <v>68</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D1" s="42" t="s">
         <v>69</v>
@@ -2555,7 +2561,7 @@
         <v>28</v>
       </c>
       <c r="M1" s="42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N1" s="42" t="s">
         <v>61</v>
@@ -2564,7 +2570,7 @@
         <v>31</v>
       </c>
       <c r="P1" s="42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q1" s="34" t="s">
         <v>75</v>
@@ -2602,8 +2608,11 @@
       <c r="AB1" s="43" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC1" s="43" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>67</v>
       </c>
@@ -2641,10 +2650,10 @@
         <v>36</v>
       </c>
       <c r="M2" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O2" s="18" t="s">
         <v>94</v>
@@ -2679,17 +2688,20 @@
       <c r="Y2" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="Z2" s="19" t="s">
-        <v>36</v>
+      <c r="Z2" s="25" t="s">
+        <v>88</v>
       </c>
       <c r="AA2" s="19" t="s">
         <v>36</v>
       </c>
       <c r="AB2" s="18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="AC2" s="25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
@@ -2774,8 +2786,11 @@
       <c r="AB3" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC3" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>70</v>
       </c>
@@ -2860,8 +2875,11 @@
       <c r="AB4" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC4" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>71</v>
       </c>
@@ -2946,8 +2964,11 @@
       <c r="AB5" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC5" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>9</v>
       </c>
@@ -2979,7 +3000,7 @@
         <v>36</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L6" s="19" t="s">
         <v>36</v>
@@ -3032,8 +3053,11 @@
       <c r="AB6" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC6" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
         <v>73</v>
       </c>
@@ -3068,7 +3092,7 @@
         <v>36</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M7" s="19" t="s">
         <v>36</v>
@@ -3118,8 +3142,11 @@
       <c r="AB7" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC7" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>72</v>
       </c>
@@ -3204,10 +3231,13 @@
       <c r="AB8" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC8" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>36</v>
@@ -3290,8 +3320,11 @@
       <c r="AB9" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC9" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
         <v>74</v>
       </c>
@@ -3314,7 +3347,7 @@
         <v>36</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I10" s="23" t="s">
         <v>92</v>
@@ -3376,35 +3409,38 @@
       <c r="AB10" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:28" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC10" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="I11" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>114</v>
-      </c>
       <c r="J11" s="19" t="s">
         <v>36</v>
       </c>
@@ -3462,8 +3498,11 @@
       <c r="AB11" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC11" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
         <v>62</v>
       </c>
@@ -3489,7 +3528,7 @@
         <v>36</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J12" s="19" t="s">
         <v>36</v>
@@ -3537,7 +3576,7 @@
         <v>36</v>
       </c>
       <c r="Y12" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Z12" s="19" t="s">
         <v>36</v>
@@ -3548,8 +3587,11 @@
       <c r="AB12" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC12" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
         <v>75</v>
       </c>
@@ -3634,8 +3676,11 @@
       <c r="AB13" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC13" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
         <v>76</v>
       </c>
@@ -3720,8 +3765,11 @@
       <c r="AB14" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC14" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
         <v>77</v>
       </c>
@@ -3806,8 +3854,11 @@
       <c r="AB15" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:28" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC15" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
         <v>78</v>
       </c>
@@ -3892,8 +3943,11 @@
       <c r="AB16" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:28" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC16" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
         <v>79</v>
       </c>
@@ -3978,8 +4032,11 @@
       <c r="AB17" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC17" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
         <v>80</v>
       </c>
@@ -4064,8 +4121,11 @@
       <c r="AB18" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC18" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
         <v>81</v>
       </c>
@@ -4150,8 +4210,11 @@
       <c r="AB19" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:28" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC19" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
         <v>82</v>
       </c>
@@ -4236,293 +4299,390 @@
       <c r="AB20" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="AC20" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="C21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="S21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="T21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="U21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="V21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="X21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC21" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="J21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="S21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="T21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="U21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="V21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="W21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="X21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB21" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
+      <c r="C22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="J22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="S22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="T22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="U22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="V22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="X22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC22" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="J23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="S23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="T23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="U23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="V23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="X23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC23" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" s="27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="F26" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" s="30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="B22" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="J22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="S22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="T22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="U22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="V22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="W22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="X22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB22" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="31"/>
-    </row>
-    <row r="24" spans="1:28" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="G24" s="27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="36" t="s">
+      <c r="E27" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="B25" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="C25" s="29" t="s">
+      <c r="G27" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="D25" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="F25" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="G25" s="30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="C26" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="D26" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="E26" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="F26" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="G26" s="33" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B27" s="20" t="s">
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B28" s="20" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="38" t="s">
+    <row r="29" spans="1:29" ht="93.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:29" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B30" s="20" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="39" t="s">
+    <row r="31" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B31" s="20" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="105" x14ac:dyDescent="0.25">
-      <c r="A31" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="B31" s="20" t="s">
+    <row r="32" spans="1:29" ht="105" x14ac:dyDescent="0.25">
+      <c r="A32" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="20" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:28" ht="90" x14ac:dyDescent="0.25">
-      <c r="A32" s="41" t="s">
+    <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A33" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B33" s="20" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
+    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B34" s="20" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ср 25.11.20 : 11:32:11,62
</commit_message>
<xml_diff>
--- a/eng.xlsx
+++ b/eng.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="129">
   <si>
     <t>Стек</t>
   </si>
@@ -405,6 +405,9 @@
   </si>
   <si>
     <t>Swap(G),Pop,getOut,Pop(BP)</t>
+  </si>
+  <si>
+    <t>Pop(NP)</t>
   </si>
 </sst>
 </file>
@@ -589,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -705,6 +708,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2501,8 +2507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3094,8 +3100,8 @@
       <c r="L7" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="M7" s="19" t="s">
-        <v>36</v>
+      <c r="M7" s="45" t="s">
+        <v>128</v>
       </c>
       <c r="N7" s="19" t="s">
         <v>36</v>
@@ -3978,8 +3984,8 @@
       <c r="J17" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="K17" s="19" t="s">
-        <v>36</v>
+      <c r="K17" s="45" t="s">
+        <v>101</v>
       </c>
       <c r="L17" s="19" t="s">
         <v>36</v>
@@ -4566,7 +4572,7 @@
       <c r="AB23" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AC23" s="16" t="s">
+      <c r="AC23" s="47" t="s">
         <v>127</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ср 25.11.20 : 12:09:20,42
</commit_message>
<xml_diff>
--- a/eng.xlsx
+++ b/eng.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="130">
   <si>
     <t>Стек</t>
   </si>
@@ -408,6 +408,9 @@
   </si>
   <si>
     <t>Pop(NP)</t>
+  </si>
+  <si>
+    <t>program</t>
   </si>
 </sst>
 </file>
@@ -2505,10 +2508,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC34"/>
+  <dimension ref="A1:AD38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2529,7 +2532,7 @@
     <col min="28" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="43" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="43" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
@@ -2617,8 +2620,11 @@
       <c r="AC1" s="43" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD1" s="43" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>67</v>
       </c>
@@ -2706,8 +2712,11 @@
       <c r="AC2" s="25" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="3" spans="1:29" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD2" s="18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
@@ -2795,8 +2804,11 @@
       <c r="AC3" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD3" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>70</v>
       </c>
@@ -2884,8 +2896,11 @@
       <c r="AC4" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD4" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>71</v>
       </c>
@@ -2973,8 +2988,11 @@
       <c r="AC5" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD5" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>9</v>
       </c>
@@ -3062,8 +3080,11 @@
       <c r="AC6" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:29" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD6" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
         <v>73</v>
       </c>
@@ -3151,8 +3172,11 @@
       <c r="AC7" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD7" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>72</v>
       </c>
@@ -3240,8 +3264,11 @@
       <c r="AC8" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:29" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD8" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
         <v>124</v>
       </c>
@@ -3329,8 +3356,11 @@
       <c r="AC9" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:29" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD9" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
         <v>74</v>
       </c>
@@ -3418,8 +3448,11 @@
       <c r="AC10" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:29" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD10" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
         <v>112</v>
       </c>
@@ -3507,8 +3540,11 @@
       <c r="AC11" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD11" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
         <v>62</v>
       </c>
@@ -3596,8 +3632,11 @@
       <c r="AC12" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD12" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
         <v>75</v>
       </c>
@@ -3685,8 +3724,11 @@
       <c r="AC13" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD13" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
         <v>76</v>
       </c>
@@ -3774,8 +3816,11 @@
       <c r="AC14" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:29" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD14" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
         <v>77</v>
       </c>
@@ -3863,8 +3908,11 @@
       <c r="AC15" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:29" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD15" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
         <v>78</v>
       </c>
@@ -3952,8 +4000,11 @@
       <c r="AC16" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:29" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD16" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
         <v>79</v>
       </c>
@@ -4041,8 +4092,11 @@
       <c r="AC17" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD17" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
         <v>80</v>
       </c>
@@ -4130,8 +4184,11 @@
       <c r="AC18" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:29" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD18" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
         <v>81</v>
       </c>
@@ -4219,8 +4276,11 @@
       <c r="AC19" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:29" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD19" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
         <v>82</v>
       </c>
@@ -4308,8 +4368,11 @@
       <c r="AC20" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+      <c r="AD20" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
         <v>107</v>
       </c>
@@ -4397,8 +4460,11 @@
       <c r="AC21" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:29" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD21" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
         <v>115</v>
       </c>
@@ -4486,8 +4552,11 @@
       <c r="AC22" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="23" spans="1:29" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD22" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
         <v>83</v>
       </c>
@@ -4575,120 +4644,214 @@
       <c r="AC23" s="47" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="24" spans="1:29" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:29" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
+      <c r="AD23" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I24" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="J24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="S24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="T24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="U24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="V24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="X24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD24" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B27" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C27" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="D27" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="26" t="s">
+      <c r="E27" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="F27" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="G25" s="27" t="s">
+      <c r="G27" s="27" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:29" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="36" t="s">
+    <row r="28" spans="1:30" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B28" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C28" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="D26" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26" s="29" t="s">
+      <c r="D28" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="F26" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="G26" s="30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:29" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="37" t="s">
+      <c r="F28" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G28" s="30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B29" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C29" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="31" t="s">
+      <c r="D29" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="E27" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27" s="20" t="s">
+      <c r="E29" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="G27" s="33" t="s">
+      <c r="G29" s="33" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B28" s="20" t="s">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B30" s="20" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:29" ht="93.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:29" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" s="38" t="s">
+    <row r="34" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B34" s="20" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:29" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="39" t="s">
+    <row r="35" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B35" s="20" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:29" ht="105" x14ac:dyDescent="0.25">
-      <c r="A32" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="B32" s="20" t="s">
+    <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A36" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" s="20" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A33" s="41" t="s">
+    <row r="37" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A37" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B37" s="20" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="34" t="s">
+    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B38" s="20" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ср 25.11.20 : 12:30:56,81
</commit_message>
<xml_diff>
--- a/eng.xlsx
+++ b/eng.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="131">
   <si>
     <t>Стек</t>
   </si>
@@ -411,13 +411,29 @@
   </si>
   <si>
     <t>program</t>
+  </si>
+  <si>
+    <r>
+      <t>Pop,getOut,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>endF</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,6 +445,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -2511,7 +2535,7 @@
   <dimension ref="A1:AD38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2916,8 +2940,8 @@
       <c r="E5" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F5" s="22" t="s">
-        <v>89</v>
+      <c r="F5" s="45" t="s">
+        <v>130</v>
       </c>
       <c r="G5" s="19" t="s">
         <v>36</v>
@@ -4857,5 +4881,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ср 25.11.20 : 13:22:54,51
</commit_message>
<xml_diff>
--- a/eng.xlsx
+++ b/eng.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="133">
   <si>
     <t>Стек</t>
   </si>
@@ -427,6 +427,12 @@
       </rPr>
       <t>endF</t>
     </r>
+  </si>
+  <si>
+    <t>f(2,w)</t>
+  </si>
+  <si>
+    <t>F2</t>
   </si>
 </sst>
 </file>
@@ -2534,8 +2540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2928,13 +2934,13 @@
       <c r="A5" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="45" t="s">
         <v>98</v>
       </c>
       <c r="E5" s="18" t="s">
@@ -4787,8 +4793,11 @@
       <c r="G27" s="27" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="28" spans="1:30" ht="45" x14ac:dyDescent="0.25">
+      <c r="I27" s="20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="36" t="s">
         <v>117</v>
       </c>
@@ -4807,8 +4816,11 @@
       <c r="F28" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="G28" s="30" t="s">
-        <v>36</v>
+      <c r="G28" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="I28" s="20" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:30" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Ср 25.11.20 : 13:57:22,64
</commit_message>
<xml_diff>
--- a/eng.xlsx
+++ b/eng.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="138">
   <si>
     <t>Стек</t>
   </si>
@@ -433,6 +433,34 @@
   </si>
   <si>
     <t>F2</t>
+  </si>
+  <si>
+    <t>var</t>
+  </si>
+  <si>
+    <t>var (perem)</t>
+  </si>
+  <si>
+    <t>Push(perem_0)</t>
+  </si>
+  <si>
+    <t>Swap(perem_i+1)</t>
+  </si>
+  <si>
+    <r>
+      <t>Pop(X),getOut,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>endType</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2538,10 +2566,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD38"/>
+  <dimension ref="A1:AE38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2562,7 +2590,7 @@
     <col min="28" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="43" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" s="43" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
@@ -2653,8 +2681,11 @@
       <c r="AD1" s="43" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE1" s="43" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>67</v>
       </c>
@@ -2745,8 +2776,11 @@
       <c r="AD2" s="18" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE2" s="18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
@@ -2837,8 +2871,11 @@
       <c r="AD3" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:30" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE3" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>70</v>
       </c>
@@ -2929,8 +2966,11 @@
       <c r="AD4" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:30" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE4" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>71</v>
       </c>
@@ -3021,8 +3061,11 @@
       <c r="AD5" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:30" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE5" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>9</v>
       </c>
@@ -3113,8 +3156,11 @@
       <c r="AD6" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:30" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE6" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
         <v>73</v>
       </c>
@@ -3205,8 +3251,11 @@
       <c r="AD7" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE7" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>72</v>
       </c>
@@ -3297,8 +3346,11 @@
       <c r="AD8" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:30" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE8" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
         <v>124</v>
       </c>
@@ -3389,8 +3441,11 @@
       <c r="AD9" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:30" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE9" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
         <v>74</v>
       </c>
@@ -3481,8 +3536,11 @@
       <c r="AD10" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:30" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE10" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
         <v>112</v>
       </c>
@@ -3573,8 +3631,11 @@
       <c r="AD11" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE11" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
         <v>62</v>
       </c>
@@ -3665,8 +3726,11 @@
       <c r="AD12" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE12" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
         <v>75</v>
       </c>
@@ -3757,8 +3821,11 @@
       <c r="AD13" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE13" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
         <v>76</v>
       </c>
@@ -3849,8 +3916,11 @@
       <c r="AD14" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:30" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE14" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
         <v>77</v>
       </c>
@@ -3941,8 +4011,11 @@
       <c r="AD15" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:30" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE15" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
         <v>78</v>
       </c>
@@ -4033,8 +4106,11 @@
       <c r="AD16" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:30" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE16" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
         <v>79</v>
       </c>
@@ -4125,8 +4201,11 @@
       <c r="AD17" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE17" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
         <v>80</v>
       </c>
@@ -4217,8 +4296,11 @@
       <c r="AD18" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:30" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE18" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
         <v>81</v>
       </c>
@@ -4309,8 +4391,11 @@
       <c r="AD19" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:30" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE19" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
         <v>82</v>
       </c>
@@ -4401,8 +4486,11 @@
       <c r="AD20" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="AE20" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
         <v>107</v>
       </c>
@@ -4493,8 +4581,11 @@
       <c r="AD21" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:30" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE21" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
         <v>115</v>
       </c>
@@ -4585,8 +4676,11 @@
       <c r="AD22" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="23" spans="1:30" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE22" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
         <v>83</v>
       </c>
@@ -4677,8 +4771,11 @@
       <c r="AD23" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="1:30" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE23" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
         <v>129</v>
       </c>
@@ -4769,9 +4866,107 @@
       <c r="AD24" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="AE24" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="I25" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="J25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P25" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="S25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="T25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="U25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="V25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="X25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z25" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE25" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="35" t="s">
         <v>0</v>
       </c>
@@ -4797,7 +4992,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="1:30" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="36" t="s">
         <v>117</v>
       </c>
@@ -4823,7 +5018,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="1:30" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="37" t="s">
         <v>64</v>
       </c>
@@ -4846,7 +5041,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B30" s="20" t="s">
         <v>93</v>
       </c>

</xml_diff>

<commit_message>
Чт 26.11.20 : 17:20:56,04
</commit_message>
<xml_diff>
--- a/eng.xlsx
+++ b/eng.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="137">
   <si>
     <t>Стек</t>
   </si>
@@ -413,22 +413,6 @@
     <t>program</t>
   </si>
   <si>
-    <r>
-      <t>Pop,getOut,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>endF</t>
-    </r>
-  </si>
-  <si>
     <t>f(2,w)</t>
   </si>
   <si>
@@ -447,20 +431,7 @@
     <t>Swap(perem_i+1)</t>
   </si>
   <si>
-    <r>
-      <t>Pop(X),getOut,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>endType</t>
-    </r>
+    <t>Pop(X),getOut</t>
   </si>
 </sst>
 </file>
@@ -486,14 +457,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -557,6 +526,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -653,7 +628,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -772,6 +747,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2568,8 +2546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2682,7 +2660,7 @@
         <v>129</v>
       </c>
       <c r="AE1" s="43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2713,7 +2691,7 @@
       <c r="I2" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="48" t="s">
         <v>95</v>
       </c>
       <c r="K2" s="19" t="s">
@@ -2777,7 +2755,7 @@
         <v>94</v>
       </c>
       <c r="AE2" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2987,7 +2965,7 @@
         <v>94</v>
       </c>
       <c r="F5" s="45" t="s">
-        <v>130</v>
+        <v>89</v>
       </c>
       <c r="G5" s="19" t="s">
         <v>36</v>
@@ -4870,9 +4848,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>36</v>
@@ -4893,7 +4871,7 @@
         <v>36</v>
       </c>
       <c r="H25" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I25" s="45" t="s">
         <v>89</v>
@@ -4917,7 +4895,7 @@
         <v>36</v>
       </c>
       <c r="P25" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q25" s="19" t="s">
         <v>36</v>
@@ -4989,7 +4967,7 @@
         <v>63</v>
       </c>
       <c r="I27" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:31" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5015,7 +4993,7 @@
         <v>102</v>
       </c>
       <c r="I28" s="20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:31" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Чт 26.11.20 : 20:49:54,65
</commit_message>
<xml_diff>
--- a/eng.xlsx
+++ b/eng.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="139">
   <si>
     <t>Стек</t>
   </si>
@@ -238,12 +238,6 @@
     <t>Fi</t>
   </si>
   <si>
-    <t xml:space="preserve">IF_mi+1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF_mi </t>
-  </si>
-  <si>
     <t xml:space="preserve">D_i,j,k </t>
   </si>
   <si>
@@ -292,9 +286,6 @@
     <t>Pop,getOut</t>
   </si>
   <si>
-    <t>Pop(Mi:),getOut</t>
-  </si>
-  <si>
     <t>Pop(Mi+1:),getOut</t>
   </si>
   <si>
@@ -338,9 +329,6 @@
   </si>
   <si>
     <t>Pop(X),Swap(2F),State(0)</t>
-  </si>
-  <si>
-    <t>Pop(Mi+1_BP_Mi:), Swap(Mi+1_IF)</t>
   </si>
   <si>
     <t>BP</t>
@@ -365,9 +353,6 @@
     <t>Pop(k_type),getOut,Hold</t>
   </si>
   <si>
-    <t>Pop(Mi_UPL),Swap(Mi_IF)</t>
-  </si>
-  <si>
     <t>UPL</t>
   </si>
   <si>
@@ -407,9 +392,6 @@
     <t>Swap(G),Pop,getOut,Pop(BP)</t>
   </si>
   <si>
-    <t>Pop(NP)</t>
-  </si>
-  <si>
     <t>program</t>
   </si>
   <si>
@@ -432,6 +414,30 @@
   </si>
   <si>
     <t>Pop(X),getOut</t>
+  </si>
+  <si>
+    <t>Pop(UPL_Mi_1),Swap(IF_Mi_1)</t>
+  </si>
+  <si>
+    <t>IF_Mi_x</t>
+  </si>
+  <si>
+    <t>IF_Mi+1_x</t>
+  </si>
+  <si>
+    <t>Pop(IF_Mi_i =&gt; Mi:_i),getOut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">НП должно писаться и храниться в стеке, и при натыкании на КП исчезать </t>
+  </si>
+  <si>
+    <t>KP()</t>
+  </si>
+  <si>
+    <t>Pop(NP),Push</t>
+  </si>
+  <si>
+    <t>Pop(Mi+1_BP_Mi:),Swap(Mi+1_IF)</t>
   </si>
 </sst>
 </file>
@@ -531,7 +537,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -628,7 +634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -750,6 +756,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2544,10 +2553,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE38"/>
+  <dimension ref="A1:AE45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2558,9 +2567,9 @@
     <col min="5" max="5" width="10.7109375" style="20" customWidth="1"/>
     <col min="6" max="7" width="9.140625" style="20"/>
     <col min="8" max="8" width="15.42578125" style="20" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="20" customWidth="1"/>
+    <col min="9" max="9" width="17" style="20" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="20"/>
-    <col min="11" max="11" width="13" style="20" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="20" customWidth="1"/>
     <col min="12" max="12" width="17.140625" style="20" customWidth="1"/>
     <col min="13" max="24" width="9.140625" style="20"/>
     <col min="25" max="26" width="9.140625" style="16"/>
@@ -2576,7 +2585,7 @@
         <v>68</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D1" s="42" t="s">
         <v>69</v>
@@ -2606,7 +2615,7 @@
         <v>28</v>
       </c>
       <c r="M1" s="42" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="N1" s="42" t="s">
         <v>61</v>
@@ -2615,31 +2624,31 @@
         <v>31</v>
       </c>
       <c r="P1" s="42" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="Q1" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="R1" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="S1" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="T1" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="S1" s="34" t="s">
+      <c r="U1" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="T1" s="34" t="s">
+      <c r="V1" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="U1" s="34" t="s">
+      <c r="W1" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="V1" s="34" t="s">
+      <c r="X1" s="34" t="s">
         <v>80</v>
-      </c>
-      <c r="W1" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="X1" s="34" t="s">
-        <v>82</v>
       </c>
       <c r="Y1" s="43" t="s">
         <v>58</v>
@@ -2651,16 +2660,16 @@
         <v>4</v>
       </c>
       <c r="AB1" s="43" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AC1" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD1" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="AE1" s="43" t="s">
         <v>126</v>
-      </c>
-      <c r="AD1" s="43" t="s">
-        <v>129</v>
-      </c>
-      <c r="AE1" s="43" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2668,16 +2677,16 @@
         <v>67</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>36</v>
@@ -2692,7 +2701,7 @@
         <v>40</v>
       </c>
       <c r="J2" s="48" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K2" s="19" t="s">
         <v>36</v>
@@ -2701,61 +2710,61 @@
         <v>36</v>
       </c>
       <c r="M2" s="20" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="N2" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="V2" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="W2" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="X2" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y2" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z2" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA2" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="O2" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="P2" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="R2" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="S2" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="T2" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="U2" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="V2" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="W2" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="X2" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y2" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z2" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA2" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB2" s="18" t="s">
-        <v>125</v>
-      </c>
       <c r="AC2" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AD2" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="AE2" s="18" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2763,19 +2772,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G3" s="19" t="s">
         <v>36</v>
@@ -2811,25 +2820,25 @@
         <v>36</v>
       </c>
       <c r="R3" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="S3" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="T3" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="U3" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="V3" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="W3" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X3" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Y3" s="19" t="s">
         <v>36</v>
@@ -2858,25 +2867,25 @@
         <v>70</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>36</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I4" s="19" t="s">
         <v>36</v>
@@ -2906,25 +2915,25 @@
         <v>36</v>
       </c>
       <c r="R4" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="S4" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="T4" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="U4" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="V4" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="W4" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X4" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Y4" s="19" t="s">
         <v>36</v>
@@ -2953,25 +2962,25 @@
         <v>71</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F5" s="45" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G5" s="19" t="s">
         <v>36</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I5" s="19" t="s">
         <v>36</v>
@@ -3001,25 +3010,25 @@
         <v>36</v>
       </c>
       <c r="R5" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="S5" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="T5" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="U5" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="V5" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="W5" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X5" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Y5" s="19" t="s">
         <v>36</v>
@@ -3048,16 +3057,16 @@
         <v>9</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>36</v>
@@ -3074,8 +3083,8 @@
       <c r="J6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="K6" s="23" t="s">
-        <v>114</v>
+      <c r="K6" s="49" t="s">
+        <v>131</v>
       </c>
       <c r="L6" s="19" t="s">
         <v>36</v>
@@ -3096,25 +3105,25 @@
         <v>36</v>
       </c>
       <c r="R6" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="S6" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="T6" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="U6" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="V6" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="W6" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X6" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Y6" s="19" t="s">
         <v>36</v>
@@ -3140,19 +3149,19 @@
     </row>
     <row r="7" spans="1:31" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
-        <v>73</v>
+        <v>132</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>36</v>
@@ -3163,20 +3172,20 @@
       <c r="H7" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="20" t="s">
-        <v>90</v>
+      <c r="I7" s="49" t="s">
+        <v>134</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K7" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="L7" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="M7" s="45" t="s">
-        <v>128</v>
+      <c r="L7" s="49" t="s">
+        <v>138</v>
+      </c>
+      <c r="M7" s="49" t="s">
+        <v>137</v>
       </c>
       <c r="N7" s="19" t="s">
         <v>36</v>
@@ -3188,28 +3197,28 @@
         <v>36</v>
       </c>
       <c r="Q7" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="R7" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="S7" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="T7" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="U7" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="V7" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="W7" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X7" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Y7" s="19" t="s">
         <v>36</v>
@@ -3235,40 +3244,40 @@
     </row>
     <row r="8" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
-        <v>72</v>
+        <v>133</v>
       </c>
       <c r="B8" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" s="20" t="s">
-        <v>91</v>
-      </c>
       <c r="J8" s="20" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K8" s="19" t="s">
         <v>36</v>
       </c>
       <c r="L8" s="20" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M8" s="19" t="s">
         <v>36</v>
@@ -3283,28 +3292,28 @@
         <v>36</v>
       </c>
       <c r="Q8" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="R8" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="S8" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="T8" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="U8" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="V8" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="W8" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X8" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Y8" s="19" t="s">
         <v>36</v>
@@ -3330,7 +3339,7 @@
     </row>
     <row r="9" spans="1:31" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>36</v>
@@ -3339,10 +3348,10 @@
         <v>36</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F9" s="19" t="s">
         <v>36</v>
@@ -3354,7 +3363,7 @@
         <v>36</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J9" s="19" t="s">
         <v>36</v>
@@ -3425,7 +3434,7 @@
     </row>
     <row r="10" spans="1:31" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>36</v>
@@ -3434,7 +3443,7 @@
         <v>36</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>40</v>
@@ -3446,10 +3455,10 @@
         <v>36</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J10" s="19" t="s">
         <v>36</v>
@@ -3470,7 +3479,7 @@
         <v>36</v>
       </c>
       <c r="P10" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Q10" s="19" t="s">
         <v>36</v>
@@ -3520,7 +3529,7 @@
     </row>
     <row r="11" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>36</v>
@@ -3541,10 +3550,10 @@
         <v>36</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J11" s="19" t="s">
         <v>36</v>
@@ -3639,7 +3648,7 @@
         <v>36</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="J12" s="19" t="s">
         <v>36</v>
@@ -3687,7 +3696,7 @@
         <v>36</v>
       </c>
       <c r="Y12" s="16" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="Z12" s="19" t="s">
         <v>36</v>
@@ -3710,19 +3719,19 @@
     </row>
     <row r="13" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>36</v>
@@ -3734,7 +3743,7 @@
         <v>36</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J13" s="19" t="s">
         <v>36</v>
@@ -3743,7 +3752,7 @@
         <v>36</v>
       </c>
       <c r="L13" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M13" s="19" t="s">
         <v>36</v>
@@ -3761,25 +3770,25 @@
         <v>36</v>
       </c>
       <c r="R13" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="S13" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="T13" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="U13" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="V13" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="W13" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X13" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Y13" s="19" t="s">
         <v>36</v>
@@ -3805,31 +3814,31 @@
     </row>
     <row r="14" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I14" s="45" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J14" s="19" t="s">
         <v>36</v>
@@ -3856,25 +3865,25 @@
         <v>36</v>
       </c>
       <c r="R14" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="S14" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="T14" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="U14" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="V14" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="W14" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X14" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Y14" s="19" t="s">
         <v>36</v>
@@ -3900,31 +3909,31 @@
     </row>
     <row r="15" spans="1:31" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I15" s="45" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J15" s="19" t="s">
         <v>36</v>
@@ -3951,25 +3960,25 @@
         <v>36</v>
       </c>
       <c r="R15" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="S15" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="T15" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="U15" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="V15" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="W15" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X15" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Y15" s="19" t="s">
         <v>36</v>
@@ -3995,31 +4004,31 @@
     </row>
     <row r="16" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J16" s="19" t="s">
         <v>36</v>
@@ -4046,25 +4055,25 @@
         <v>36</v>
       </c>
       <c r="R16" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="S16" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="T16" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="U16" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="V16" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="W16" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X16" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Y16" s="19" t="s">
         <v>36</v>
@@ -4090,37 +4099,37 @@
     </row>
     <row r="17" spans="1:31" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J17" s="19" t="s">
         <v>36</v>
       </c>
       <c r="K17" s="45" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="L17" s="19" t="s">
         <v>36</v>
@@ -4141,25 +4150,25 @@
         <v>36</v>
       </c>
       <c r="R17" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="S17" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="T17" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="U17" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="V17" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="W17" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X17" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Y17" s="19" t="s">
         <v>36</v>
@@ -4185,31 +4194,31 @@
     </row>
     <row r="18" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H18" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J18" s="19" t="s">
         <v>36</v>
@@ -4236,25 +4245,25 @@
         <v>36</v>
       </c>
       <c r="R18" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="S18" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="T18" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="U18" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="V18" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="W18" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X18" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Y18" s="19" t="s">
         <v>36</v>
@@ -4280,31 +4289,31 @@
     </row>
     <row r="19" spans="1:31" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H19" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J19" s="19" t="s">
         <v>36</v>
@@ -4331,25 +4340,25 @@
         <v>36</v>
       </c>
       <c r="R19" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="S19" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="T19" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="U19" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="V19" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="W19" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="X19" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>36</v>
@@ -4375,31 +4384,31 @@
     </row>
     <row r="20" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J20" s="19" t="s">
         <v>36</v>
@@ -4426,25 +4435,25 @@
         <v>36</v>
       </c>
       <c r="R20" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="S20" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="T20" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="U20" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="V20" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="W20" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="X20" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="Y20" s="19" t="s">
         <v>36</v>
@@ -4470,10 +4479,10 @@
     </row>
     <row r="21" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C21" s="19" t="s">
         <v>36</v>
@@ -4565,10 +4574,10 @@
     </row>
     <row r="22" spans="1:31" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C22" s="19" t="s">
         <v>36</v>
@@ -4660,7 +4669,7 @@
     </row>
     <row r="23" spans="1:31" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>36</v>
@@ -4744,7 +4753,7 @@
         <v>36</v>
       </c>
       <c r="AC23" s="47" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="AD23" s="19" t="s">
         <v>36</v>
@@ -4755,7 +4764,7 @@
     </row>
     <row r="24" spans="1:31" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>36</v>
@@ -4764,7 +4773,7 @@
         <v>36</v>
       </c>
       <c r="D24" s="45" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>36</v>
@@ -4779,7 +4788,7 @@
         <v>36</v>
       </c>
       <c r="I24" s="45" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J24" s="19" t="s">
         <v>36</v>
@@ -4850,7 +4859,7 @@
     </row>
     <row r="25" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="34" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>36</v>
@@ -4859,7 +4868,7 @@
         <v>36</v>
       </c>
       <c r="D25" s="45" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E25" s="19" t="s">
         <v>36</v>
@@ -4871,196 +4880,201 @@
         <v>36</v>
       </c>
       <c r="H25" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="I25" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="J25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P25" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="S25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="T25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="U25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="V25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="X25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z25" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE25" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="I25" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="J25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P25" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="S25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="T25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="U25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="V25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="W25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="X25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z25" s="23" t="s">
+    </row>
+    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="G34" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="I34" s="20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="F35" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G35" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="I35" s="20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="AA25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE25" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:31" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="26" t="s">
+      <c r="D36" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="E36" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="G36" s="33" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A41" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="F27" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="G27" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="I27" s="20" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="28" spans="1:31" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="B28" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="D28" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="F28" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="G28" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="I28" s="20" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="29" spans="1:31" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="C29" s="31" t="s">
+    </row>
+    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="D29" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="E29" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="G29" s="33" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B30" s="20" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="B34" s="20" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="39" t="s">
-        <v>99</v>
-      </c>
-      <c r="B35" s="20" t="s">
+      <c r="B42" s="20" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A36" s="40" t="s">
+    <row r="43" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A43" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B36" s="20" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A37" s="41" t="s">
+    </row>
+    <row r="44" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A44" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="B37" s="20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="34" t="s">
+    </row>
+    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B45" s="20" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Чт 26.11.20 : 22:42:49,01
</commit_message>
<xml_diff>
--- a/eng.xlsx
+++ b/eng.xlsx
@@ -419,12 +419,6 @@
     <t>Pop(UPL_Mi_1),Swap(IF_Mi_1)</t>
   </si>
   <si>
-    <t>IF_Mi_x</t>
-  </si>
-  <si>
-    <t>IF_Mi+1_x</t>
-  </si>
-  <si>
     <t>Pop(IF_Mi_i =&gt; Mi:_i),getOut</t>
   </si>
   <si>
@@ -438,6 +432,12 @@
   </si>
   <si>
     <t>Pop(Mi+1_BP_Mi:),Swap(Mi+1_IF)</t>
+  </si>
+  <si>
+    <t>IF_Mi_x (после then)</t>
+  </si>
+  <si>
+    <t>IF_Mi+1_x (после else)</t>
   </si>
 </sst>
 </file>
@@ -2555,8 +2555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2716,7 +2716,7 @@
         <v>115</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="P2" s="19" t="s">
         <v>36</v>
@@ -3149,7 +3149,7 @@
     </row>
     <row r="7" spans="1:31" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>86</v>
@@ -3173,7 +3173,7 @@
         <v>36</v>
       </c>
       <c r="I7" s="49" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J7" s="20" t="s">
         <v>92</v>
@@ -3182,10 +3182,10 @@
         <v>36</v>
       </c>
       <c r="L7" s="49" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M7" s="49" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="N7" s="19" t="s">
         <v>36</v>
@@ -3244,7 +3244,7 @@
     </row>
     <row r="8" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B8" s="25" t="s">
         <v>86</v>
@@ -4954,7 +4954,7 @@
     </row>
     <row r="29" spans="1:31" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Пт 27.11.20 :  0:21:11,21
</commit_message>
<xml_diff>
--- a/eng.xlsx
+++ b/eng.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="149">
   <si>
     <t>Стек</t>
   </si>
@@ -221,9 +221,6 @@
   </si>
   <si>
     <t>Отсутствие действия</t>
-  </si>
-  <si>
-    <t>Start</t>
   </si>
   <si>
     <t>N (число) N01</t>
@@ -438,6 +435,39 @@
   </si>
   <si>
     <t>IF_Mi+1_x (после else)</t>
+  </si>
+  <si>
+    <t>Пусто</t>
+  </si>
+  <si>
+    <t>procedure</t>
+  </si>
+  <si>
+    <t>Push(PROC_1_1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; </t>
+  </si>
+  <si>
+    <t>Push(FUNC_1_1)</t>
+  </si>
+  <si>
+    <t>FUNC</t>
+  </si>
+  <si>
+    <t>return</t>
+  </si>
+  <si>
+    <t>getOut,Push(X)</t>
+  </si>
+  <si>
+    <t>Pop(KF),getOut</t>
+  </si>
+  <si>
+    <t>Pop(X),Push(perem_0)</t>
+  </si>
+  <si>
+    <t>Pop(X),Pop(i_j_NP)</t>
   </si>
 </sst>
 </file>
@@ -468,7 +498,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -538,6 +568,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -634,7 +670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -760,6 +796,18 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2553,10 +2601,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE45"/>
+  <dimension ref="A1:AH45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2564,31 +2612,34 @@
     <col min="1" max="1" width="13" style="34" customWidth="1"/>
     <col min="2" max="2" width="11" style="20" customWidth="1"/>
     <col min="4" max="4" width="9" style="20" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="20" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="20" customWidth="1"/>
     <col min="6" max="7" width="9.140625" style="20"/>
     <col min="8" max="8" width="15.42578125" style="20" customWidth="1"/>
     <col min="9" max="9" width="17" style="20" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="20"/>
     <col min="11" max="11" width="14.5703125" style="20" customWidth="1"/>
     <col min="12" max="12" width="17.140625" style="20" customWidth="1"/>
-    <col min="13" max="24" width="9.140625" style="20"/>
+    <col min="13" max="13" width="12.42578125" style="20" customWidth="1"/>
+    <col min="14" max="24" width="9.140625" style="20"/>
     <col min="25" max="26" width="9.140625" style="16"/>
     <col min="27" max="27" width="9.140625" style="20"/>
-    <col min="28" max="16384" width="9.140625" style="16"/>
+    <col min="28" max="31" width="9.140625" style="16"/>
+    <col min="32" max="32" width="10.28515625" style="16" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="43" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="43" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="42" t="s">
         <v>68</v>
-      </c>
-      <c r="C1" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>69</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>2</v>
@@ -2603,7 +2654,7 @@
         <v>24</v>
       </c>
       <c r="I1" s="42" t="s">
-        <v>25</v>
+        <v>141</v>
       </c>
       <c r="J1" s="42" t="s">
         <v>26</v>
@@ -2615,7 +2666,7 @@
         <v>28</v>
       </c>
       <c r="M1" s="42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N1" s="42" t="s">
         <v>61</v>
@@ -2624,31 +2675,31 @@
         <v>31</v>
       </c>
       <c r="P1" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q1" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="R1" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="S1" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="S1" s="34" t="s">
+      <c r="T1" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="T1" s="34" t="s">
+      <c r="U1" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="U1" s="34" t="s">
+      <c r="V1" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="V1" s="34" t="s">
+      <c r="W1" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="W1" s="34" t="s">
+      <c r="X1" s="34" t="s">
         <v>79</v>
-      </c>
-      <c r="X1" s="34" t="s">
-        <v>80</v>
       </c>
       <c r="Y1" s="43" t="s">
         <v>58</v>
@@ -2660,33 +2711,42 @@
         <v>4</v>
       </c>
       <c r="AB1" s="43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AC1" s="43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AD1" s="43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AE1" s="43" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="AF1" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="AG1" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH1" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>67</v>
+        <v>138</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>36</v>
@@ -2701,7 +2761,7 @@
         <v>40</v>
       </c>
       <c r="J2" s="48" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K2" s="19" t="s">
         <v>36</v>
@@ -2710,278 +2770,305 @@
         <v>36</v>
       </c>
       <c r="M2" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P2" s="19" t="s">
         <v>36</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R2" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="S2" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T2" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="U2" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="V2" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="W2" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="X2" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Y2" s="19" t="s">
         <v>36</v>
       </c>
       <c r="Z2" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AA2" s="19" t="s">
         <v>36</v>
       </c>
       <c r="AB2" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AC2" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AD2" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AE2" s="18" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="AF2" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG2" s="51" t="s">
+        <v>142</v>
+      </c>
+      <c r="AH2" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="S3" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="T3" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="U3" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="V3" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="W3" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="X3" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG3" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH3" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="H4" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="S4" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="T4" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="U4" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="V4" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="W4" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="X4" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG4" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH4" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R3" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="S3" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="T3" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="U3" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="V3" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="W3" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="X3" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE3" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="H4" s="20" t="s">
+      <c r="G5" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="I4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R4" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="S4" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="T4" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="U4" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="V4" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="W4" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="X4" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE4" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="45" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F5" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>101</v>
-      </c>
       <c r="I5" s="19" t="s">
         <v>36</v>
       </c>
@@ -3010,25 +3097,25 @@
         <v>36</v>
       </c>
       <c r="R5" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="S5" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T5" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="U5" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="V5" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="W5" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="X5" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Y5" s="19" t="s">
         <v>36</v>
@@ -3051,320 +3138,356 @@
       <c r="AE5" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:31" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF5" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG5" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH5" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R6" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="S6" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="T6" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="U6" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="V6" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="W6" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="X6" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG6" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH6" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="49" t="s">
+        <v>135</v>
+      </c>
+      <c r="M7" s="49" t="s">
+        <v>134</v>
+      </c>
+      <c r="N7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q7" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="R7" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="S7" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="T7" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="U7" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="V7" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="W7" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="X7" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG7" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH7" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q8" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="R8" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="S8" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="T8" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="U8" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="V8" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="W8" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="X8" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG8" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH8" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K6" s="49" t="s">
-        <v>131</v>
-      </c>
-      <c r="L6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R6" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="S6" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="T6" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="U6" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="V6" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="W6" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="X6" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE6" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="49" t="s">
-        <v>132</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L7" s="49" t="s">
-        <v>136</v>
-      </c>
-      <c r="M7" s="49" t="s">
-        <v>135</v>
-      </c>
-      <c r="N7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q7" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="R7" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="S7" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="T7" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="U7" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="V7" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="W7" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="X7" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE7" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" s="49" t="s">
-        <v>88</v>
-      </c>
-      <c r="J8" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L8" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="M8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q8" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="R8" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="S8" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="T8" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="U8" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="V8" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="W8" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="X8" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE8" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" s="22" t="s">
-        <v>87</v>
-      </c>
       <c r="J9" s="19" t="s">
         <v>36</v>
       </c>
@@ -3431,10 +3554,19 @@
       <c r="AE9" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:31" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF9" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG9" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH9" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>36</v>
@@ -3443,7 +3575,7 @@
         <v>36</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>40</v>
@@ -3455,118 +3587,127 @@
         <v>36</v>
       </c>
       <c r="H10" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="I10" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="S10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="T10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="U10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="V10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="X10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG10" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH10" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="I10" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="J10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P10" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="S10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="T10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="U10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="V10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="W10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="X10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE10" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="I11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M11" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="J11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M11" s="19" t="s">
-        <v>36</v>
-      </c>
       <c r="N11" s="19" t="s">
         <v>36</v>
       </c>
@@ -3621,8 +3762,17 @@
       <c r="AE11" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG11" s="52" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH11" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
         <v>62</v>
       </c>
@@ -3648,7 +3798,7 @@
         <v>36</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J12" s="19" t="s">
         <v>36</v>
@@ -3696,7 +3846,7 @@
         <v>36</v>
       </c>
       <c r="Y12" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Z12" s="19" t="s">
         <v>36</v>
@@ -3716,1245 +3866,1579 @@
       <c r="AE12" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF12" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG12" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH12" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L13" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="M13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R13" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="S13" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="T13" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="U13" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="V13" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="W13" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="X13" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG13" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH13" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B14" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="I14" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L14" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M14" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N14" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O14" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P14" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q14" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R14" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="S14" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="T14" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="U14" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="V14" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="W14" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="X14" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y14" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z14" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA14" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB14" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC14" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD14" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE14" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF14" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG14" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH14" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M15" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N15" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O15" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P15" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q15" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R15" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="S15" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="T15" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="U15" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="V15" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="W15" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="X15" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y15" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z15" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA15" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB15" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC15" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD15" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE15" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF15" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG15" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH15" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R16" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="S16" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="T16" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="U16" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="V16" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="W16" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="X16" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG16" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH16" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H17" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="J17" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="L17" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N17" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O17" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P17" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q17" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R17" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="S17" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="T17" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="U17" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="V17" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="W17" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="X17" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y17" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z17" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA17" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB17" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC17" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD17" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE17" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF17" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG17" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH17" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K18" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L18" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M18" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N18" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O18" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P18" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q18" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R18" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="S18" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="T18" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="U18" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="V18" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="W18" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="X18" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y18" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z18" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA18" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB18" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC18" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD18" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE18" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF18" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG18" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH18" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K19" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L19" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M19" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N19" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O19" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P19" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q19" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R19" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="S19" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="T19" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="U19" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="V19" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="W19" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="X19" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y19" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z19" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA19" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB19" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC19" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD19" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE19" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF19" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG19" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH19" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="J20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R20" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="S20" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="T20" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="U20" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="V20" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="W20" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="X20" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG20" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH20" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="S21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="T21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="U21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="V21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="X21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG21" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH21" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="J22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="S22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="T22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="U22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="V22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="X22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG22" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH22" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="J23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="S23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="T23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="U23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="V23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="X23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC23" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG23" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH23" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I24" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="J24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="S24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="T24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="U24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="V24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="X24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG24" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH24" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="I25" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I13" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="J13" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K13" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L13" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="M13" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N13" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O13" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P13" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q13" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R13" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="S13" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="T13" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="U13" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="V13" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="W13" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="X13" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y13" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z13" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA13" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB13" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC13" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD13" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE13" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="H14" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I14" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="J14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R14" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="S14" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="T14" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="U14" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="V14" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="W14" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="X14" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE14" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="H15" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I15" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="J15" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K15" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L15" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M15" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N15" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O15" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P15" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q15" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R15" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="S15" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="T15" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="U15" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="V15" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="W15" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="X15" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y15" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z15" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA15" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB15" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC15" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD15" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE15" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I16" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="J16" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K16" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L16" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M16" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N16" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O16" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P16" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q16" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R16" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="S16" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="T16" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="U16" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="V16" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="W16" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="X16" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y16" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z16" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA16" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB16" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC16" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD16" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE16" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:31" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G17" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="H17" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I17" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="J17" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K17" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="L17" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M17" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N17" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O17" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P17" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q17" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R17" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="S17" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="T17" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="U17" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="V17" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="W17" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="X17" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y17" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z17" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA17" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB17" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC17" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD17" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE17" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F18" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G18" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="H18" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I18" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="J18" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K18" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L18" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M18" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N18" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O18" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P18" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q18" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R18" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="S18" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="T18" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="U18" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="V18" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="W18" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="X18" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y18" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z18" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA18" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB18" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC18" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD18" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE18" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:31" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G19" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="H19" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I19" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="J19" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K19" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L19" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M19" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N19" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O19" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P19" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q19" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R19" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="S19" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="T19" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="U19" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="V19" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="W19" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="X19" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y19" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z19" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA19" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB19" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC19" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD19" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE19" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I20" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="J20" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K20" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L20" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M20" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N20" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O20" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P20" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q20" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R20" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="S20" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="T20" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="U20" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="V20" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="W20" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="X20" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y20" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z20" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA20" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB20" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC20" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD20" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE20" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:31" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="J21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="S21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="T21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="U21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="V21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="W21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="X21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD21" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE21" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:31" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="J22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="S22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="T22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="U22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="V22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="W22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="X22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE22" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:31" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="J23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="S23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="T23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="U23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="V23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="W23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="X23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC23" s="47" t="s">
-        <v>122</v>
-      </c>
-      <c r="AD23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE23" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:31" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I24" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="J24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="S24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="T24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="U24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="V24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="W24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="X24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE24" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:31" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
+      <c r="J25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P25" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="S25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="T25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="U25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="V25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="X25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z25" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG25" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH25" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="F26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="H26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="I26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="J26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="K26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="L26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="M26" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="N26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="O26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="P26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="R26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="S26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="T26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="U26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="V26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="W26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="X26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE26" s="52" t="s">
         <v>127</v>
       </c>
-      <c r="B25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H25" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="I25" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="J25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P25" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="S25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="T25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="U25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="V25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="W25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="X25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z25" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="AA25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE25" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:31" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG26" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH26" s="51" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="53" t="s">
+        <v>144</v>
+      </c>
+      <c r="B27" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="F27" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="I27" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="J27" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="K27" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="L27" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="M27" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="N27" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="O27" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="P27" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q27" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="R27" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="S27" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="T27" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="U27" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="V27" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="W27" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="X27" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y27" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z27" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA27" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB27" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC27" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD27" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE27" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF27" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG27" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH27" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4972,7 +5456,7 @@
         <v>4</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F34" s="20" t="s">
         <v>59</v>
@@ -4981,33 +5465,33 @@
         <v>63</v>
       </c>
       <c r="I34" s="20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="F35" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G35" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="I35" s="20" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="B35" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="D35" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="F35" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="G35" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="I35" s="20" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5015,40 +5499,40 @@
         <v>64</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E36" s="32" t="s">
         <v>36</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G36" s="33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B37" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B42" s="20" t="s">
         <v>65</v>
@@ -5056,18 +5540,18 @@
     </row>
     <row r="43" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Пт 27.11.20 : 11:42:55,20
</commit_message>
<xml_diff>
--- a/eng.xlsx
+++ b/eng.xlsx
@@ -410,9 +410,6 @@
     <t>Swap(perem_i+1)</t>
   </si>
   <si>
-    <t>Pop(X),getOut</t>
-  </si>
-  <si>
     <t>Pop(UPL_Mi_1),Swap(IF_Mi_1)</t>
   </si>
   <si>
@@ -449,25 +446,28 @@
     <t xml:space="preserve">; </t>
   </si>
   <si>
-    <t>Push(FUNC_1_1)</t>
-  </si>
-  <si>
     <t>FUNC</t>
   </si>
   <si>
     <t>return</t>
   </si>
   <si>
-    <t>getOut,Push(X)</t>
-  </si>
-  <si>
     <t>Pop(KF),getOut</t>
   </si>
   <si>
     <t>Pop(X),Push(perem_0)</t>
   </si>
   <si>
-    <t>Pop(X),Pop(i_j_NP)</t>
+    <t>Push(FUNC_i_i)</t>
+  </si>
+  <si>
+    <t>Pop(X),Pop,getOut,Push(perem_0)</t>
+  </si>
+  <si>
+    <t>getOut,Hold</t>
+  </si>
+  <si>
+    <t>Pop,getOut,Push(perem_0)</t>
   </si>
 </sst>
 </file>
@@ -573,7 +573,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -670,7 +670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -797,17 +797,20 @@
     <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2603,15 +2606,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AF25" sqref="B2:AF25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="34" customWidth="1"/>
     <col min="2" max="2" width="11" style="20" customWidth="1"/>
-    <col min="4" max="4" width="9" style="20" customWidth="1"/>
+    <col min="4" max="4" width="21" style="20" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" style="20" customWidth="1"/>
     <col min="6" max="7" width="9.140625" style="20"/>
     <col min="8" max="8" width="15.42578125" style="20" customWidth="1"/>
@@ -2625,7 +2628,8 @@
     <col min="27" max="27" width="9.140625" style="20"/>
     <col min="28" max="31" width="9.140625" style="16"/>
     <col min="32" max="32" width="10.28515625" style="16" customWidth="1"/>
-    <col min="33" max="16384" width="9.140625" style="16"/>
+    <col min="33" max="34" width="9.140625" style="51"/>
+    <col min="35" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" s="43" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2654,7 +2658,7 @@
         <v>24</v>
       </c>
       <c r="I1" s="42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J1" s="42" t="s">
         <v>26</v>
@@ -2723,18 +2727,18 @@
         <v>125</v>
       </c>
       <c r="AF1" s="43" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AG1" s="50" t="s">
         <v>30</v>
       </c>
       <c r="AH1" s="50" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:34" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>85</v>
@@ -2776,7 +2780,7 @@
         <v>114</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P2" s="19" t="s">
         <v>36</v>
@@ -2827,12 +2831,12 @@
         <v>127</v>
       </c>
       <c r="AF2" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="AG2" s="51" t="s">
-        <v>142</v>
-      </c>
-      <c r="AH2" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="AG2" s="53" t="s">
+        <v>145</v>
+      </c>
+      <c r="AH2" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2933,10 +2937,10 @@
       <c r="AF3" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG3" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH3" s="52" t="s">
+      <c r="AG3" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH3" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3037,10 +3041,10 @@
       <c r="AF4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG4" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH4" s="52" t="s">
+      <c r="AG4" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH4" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3141,10 +3145,10 @@
       <c r="AF5" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG5" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH5" s="52" t="s">
+      <c r="AG5" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH5" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3180,7 +3184,7 @@
         <v>36</v>
       </c>
       <c r="K6" s="49" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L6" s="19" t="s">
         <v>36</v>
@@ -3245,16 +3249,16 @@
       <c r="AF6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG6" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH6" s="52" t="s">
+      <c r="AG6" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH6" s="23" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:34" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>85</v>
@@ -3278,7 +3282,7 @@
         <v>36</v>
       </c>
       <c r="I7" s="49" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J7" s="20" t="s">
         <v>91</v>
@@ -3287,10 +3291,10 @@
         <v>36</v>
       </c>
       <c r="L7" s="49" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M7" s="49" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N7" s="19" t="s">
         <v>36</v>
@@ -3349,16 +3353,16 @@
       <c r="AF7" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG7" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH7" s="52" t="s">
+      <c r="AG7" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH7" s="23" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B8" s="25" t="s">
         <v>85</v>
@@ -3453,10 +3457,10 @@
       <c r="AF8" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG8" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH8" s="52" t="s">
+      <c r="AG8" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH8" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3557,10 +3561,10 @@
       <c r="AF9" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG9" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH9" s="52" t="s">
+      <c r="AG9" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH9" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3661,10 +3665,10 @@
       <c r="AF10" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG10" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH10" s="52" t="s">
+      <c r="AG10" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH10" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3765,10 +3769,10 @@
       <c r="AF11" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG11" s="52" t="s">
+      <c r="AG11" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="AH11" s="52" t="s">
+      <c r="AH11" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3869,10 +3873,10 @@
       <c r="AF12" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG12" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH12" s="52" t="s">
+      <c r="AG12" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH12" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3973,10 +3977,10 @@
       <c r="AF13" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG13" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH13" s="52" t="s">
+      <c r="AG13" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH13" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4077,10 +4081,10 @@
       <c r="AF14" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG14" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH14" s="52" t="s">
+      <c r="AG14" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH14" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4181,10 +4185,10 @@
       <c r="AF15" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG15" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH15" s="52" t="s">
+      <c r="AG15" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH15" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4285,10 +4289,10 @@
       <c r="AF16" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG16" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH16" s="52" t="s">
+      <c r="AG16" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH16" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4389,10 +4393,10 @@
       <c r="AF17" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG17" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH17" s="52" t="s">
+      <c r="AG17" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH17" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4493,10 +4497,10 @@
       <c r="AF18" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG18" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH18" s="52" t="s">
+      <c r="AG18" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH18" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4597,10 +4601,10 @@
       <c r="AF19" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG19" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH19" s="52" t="s">
+      <c r="AG19" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH19" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4701,10 +4705,10 @@
       <c r="AF20" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG20" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH20" s="52" t="s">
+      <c r="AG20" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH20" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4805,10 +4809,10 @@
       <c r="AF21" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG21" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH21" s="52" t="s">
+      <c r="AG21" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH21" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4909,10 +4913,10 @@
       <c r="AF22" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG22" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH22" s="52" t="s">
+      <c r="AG22" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH22" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5013,10 +5017,10 @@
       <c r="AF23" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG23" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH23" s="52" t="s">
+      <c r="AG23" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH23" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5117,10 +5121,10 @@
       <c r="AF24" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG24" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH24" s="52" t="s">
+      <c r="AG24" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH24" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5149,8 +5153,8 @@
       <c r="H25" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="I25" s="45" t="s">
-        <v>86</v>
+      <c r="I25" s="54" t="s">
+        <v>148</v>
       </c>
       <c r="J25" s="19" t="s">
         <v>36</v>
@@ -5161,8 +5165,8 @@
       <c r="L25" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="M25" s="19" t="s">
-        <v>36</v>
+      <c r="M25" s="54" t="s">
+        <v>147</v>
       </c>
       <c r="N25" s="19" t="s">
         <v>36</v>
@@ -5171,7 +5175,7 @@
         <v>36</v>
       </c>
       <c r="P25" s="23" t="s">
-        <v>129</v>
+        <v>85</v>
       </c>
       <c r="Q25" s="19" t="s">
         <v>36</v>
@@ -5201,7 +5205,7 @@
         <v>36</v>
       </c>
       <c r="Z25" s="23" t="s">
-        <v>89</v>
+        <v>128</v>
       </c>
       <c r="AA25" s="19" t="s">
         <v>36</v>
@@ -5221,224 +5225,224 @@
       <c r="AF25" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG25" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH25" s="52" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="53" t="s">
+      <c r="AG25" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH25" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" s="51" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="52" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="H26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="J26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="K26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="L26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="M26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="N26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="O26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="P26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="R26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="S26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="T26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="U26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="V26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="W26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="X26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH26" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" s="51" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I27" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="B26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="52" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26" s="52" t="s">
-        <v>147</v>
-      </c>
-      <c r="F26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="G26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="H26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="I26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="J26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="K26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="L26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="M26" s="52" t="s">
-        <v>148</v>
-      </c>
-      <c r="N26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="O26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="P26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="R26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="S26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="T26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="U26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="V26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="W26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="X26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE26" s="52" t="s">
-        <v>127</v>
-      </c>
-      <c r="AF26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG26" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH26" s="51" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="27" spans="1:34" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="53" t="s">
-        <v>144</v>
-      </c>
-      <c r="B27" s="52" t="s">
-        <v>85</v>
-      </c>
-      <c r="C27" s="52" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" s="52" t="s">
-        <v>94</v>
-      </c>
-      <c r="E27" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="F27" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="G27" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="H27" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="I27" s="52" t="s">
-        <v>146</v>
-      </c>
-      <c r="J27" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="K27" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="L27" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="M27" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="N27" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="O27" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="P27" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q27" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="R27" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="S27" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="T27" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="U27" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="V27" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="W27" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="X27" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y27" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z27" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA27" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB27" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC27" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD27" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE27" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF27" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG27" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH27" s="52" t="s">
+      <c r="J27" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="K27" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="L27" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="M27" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="N27" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="O27" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="P27" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q27" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="R27" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="S27" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="T27" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="U27" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="V27" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="W27" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="X27" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y27" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z27" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA27" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB27" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC27" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD27" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE27" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF27" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG27" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH27" s="23" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:34" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Пт 27.11.20 : 20:41:59,19
</commit_message>
<xml_diff>
--- a/eng.xlsx
+++ b/eng.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="146">
   <si>
     <t>Стек</t>
   </si>
@@ -356,9 +356,6 @@
     <t>Push(2A),State(0)</t>
   </si>
   <si>
-    <t>F1</t>
-  </si>
-  <si>
     <t>Pop(:),State(0)</t>
   </si>
   <si>
@@ -449,25 +446,19 @@
     <t>FUNC</t>
   </si>
   <si>
-    <t>return</t>
-  </si>
-  <si>
-    <t>Pop(KF),getOut</t>
-  </si>
-  <si>
-    <t>Pop(X),Push(perem_0)</t>
-  </si>
-  <si>
     <t>Push(FUNC_i_i)</t>
   </si>
   <si>
-    <t>Pop(X),Pop,getOut,Push(perem_0)</t>
-  </si>
-  <si>
     <t>getOut,Hold</t>
   </si>
   <si>
     <t>Pop,getOut,Push(perem_0)</t>
+  </si>
+  <si>
+    <t>F1, (</t>
+  </si>
+  <si>
+    <t>Push(1F),State(1)</t>
   </si>
 </sst>
 </file>
@@ -2606,8 +2597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF25" sqref="B2:AF25"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B2:AG26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2658,7 +2649,7 @@
         <v>24</v>
       </c>
       <c r="I1" s="42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J1" s="42" t="s">
         <v>26</v>
@@ -2670,7 +2661,7 @@
         <v>28</v>
       </c>
       <c r="M1" s="42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N1" s="42" t="s">
         <v>61</v>
@@ -2718,27 +2709,25 @@
         <v>80</v>
       </c>
       <c r="AC1" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AD1" s="43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AE1" s="43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AF1" s="43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AG1" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="50" t="s">
-        <v>142</v>
-      </c>
+      <c r="AH1" s="50"/>
     </row>
     <row r="2" spans="1:34" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>85</v>
@@ -2774,13 +2763,13 @@
         <v>36</v>
       </c>
       <c r="M2" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P2" s="19" t="s">
         <v>36</v>
@@ -2819,7 +2808,7 @@
         <v>36</v>
       </c>
       <c r="AB2" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AC2" s="25" t="s">
         <v>85</v>
@@ -2828,17 +2817,15 @@
         <v>90</v>
       </c>
       <c r="AE2" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF2" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AG2" s="53" t="s">
-        <v>145</v>
-      </c>
-      <c r="AH2" s="23" t="s">
-        <v>36</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="AH2" s="23"/>
     </row>
     <row r="3" spans="1:34" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
@@ -2940,9 +2927,7 @@
       <c r="AG3" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH3" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH3" s="23"/>
     </row>
     <row r="4" spans="1:34" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
@@ -3044,9 +3029,7 @@
       <c r="AG4" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH4" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH4" s="23"/>
     </row>
     <row r="5" spans="1:34" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
@@ -3061,8 +3044,8 @@
       <c r="D5" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>90</v>
+      <c r="E5" s="29" t="s">
+        <v>145</v>
       </c>
       <c r="F5" s="45" t="s">
         <v>86</v>
@@ -3148,9 +3131,7 @@
       <c r="AG5" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH5" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH5" s="23"/>
     </row>
     <row r="6" spans="1:34" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
@@ -3184,7 +3165,7 @@
         <v>36</v>
       </c>
       <c r="K6" s="49" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L6" s="19" t="s">
         <v>36</v>
@@ -3252,13 +3233,11 @@
       <c r="AG6" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH6" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH6" s="23"/>
     </row>
     <row r="7" spans="1:34" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>85</v>
@@ -3282,7 +3261,7 @@
         <v>36</v>
       </c>
       <c r="I7" s="49" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J7" s="20" t="s">
         <v>91</v>
@@ -3291,10 +3270,10 @@
         <v>36</v>
       </c>
       <c r="L7" s="49" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M7" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N7" s="19" t="s">
         <v>36</v>
@@ -3356,13 +3335,11 @@
       <c r="AG7" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH7" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH7" s="23"/>
     </row>
     <row r="8" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B8" s="25" t="s">
         <v>85</v>
@@ -3460,13 +3437,11 @@
       <c r="AG8" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH8" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH8" s="23"/>
     </row>
     <row r="9" spans="1:34" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>36</v>
@@ -3564,9 +3539,7 @@
       <c r="AG9" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH9" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH9" s="23"/>
     </row>
     <row r="10" spans="1:34" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
@@ -3591,7 +3564,7 @@
         <v>36</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I10" s="23" t="s">
         <v>88</v>
@@ -3668,9 +3641,7 @@
       <c r="AG10" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH10" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH10" s="23"/>
     </row>
     <row r="11" spans="1:34" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
@@ -3695,7 +3666,7 @@
         <v>36</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I11" s="20" t="s">
         <v>40</v>
@@ -3772,9 +3743,7 @@
       <c r="AG11" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="AH11" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH11" s="23"/>
     </row>
     <row r="12" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
@@ -3876,9 +3845,7 @@
       <c r="AG12" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH12" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH12" s="23"/>
     </row>
     <row r="13" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
@@ -3980,9 +3947,7 @@
       <c r="AG13" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH13" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH13" s="23"/>
     </row>
     <row r="14" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
@@ -4084,9 +4049,7 @@
       <c r="AG14" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH14" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH14" s="23"/>
     </row>
     <row r="15" spans="1:34" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
@@ -4188,9 +4151,7 @@
       <c r="AG15" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH15" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH15" s="23"/>
     </row>
     <row r="16" spans="1:34" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
@@ -4292,9 +4253,7 @@
       <c r="AG16" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH16" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH16" s="23"/>
     </row>
     <row r="17" spans="1:34" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
@@ -4396,9 +4355,7 @@
       <c r="AG17" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH17" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH17" s="23"/>
     </row>
     <row r="18" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
@@ -4500,9 +4457,7 @@
       <c r="AG18" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH18" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH18" s="23"/>
     </row>
     <row r="19" spans="1:34" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
@@ -4604,9 +4559,7 @@
       <c r="AG19" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH19" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH19" s="23"/>
     </row>
     <row r="20" spans="1:34" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
@@ -4708,9 +4661,7 @@
       <c r="AG20" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH20" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH20" s="23"/>
     </row>
     <row r="21" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
@@ -4812,9 +4763,7 @@
       <c r="AG21" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH21" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH21" s="23"/>
     </row>
     <row r="22" spans="1:34" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
@@ -4916,9 +4865,7 @@
       <c r="AG22" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH22" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH22" s="23"/>
     </row>
     <row r="23" spans="1:34" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
@@ -5006,7 +4953,7 @@
         <v>36</v>
       </c>
       <c r="AC23" s="47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AD23" s="19" t="s">
         <v>36</v>
@@ -5020,13 +4967,11 @@
       <c r="AG23" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH23" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH23" s="23"/>
     </row>
     <row r="24" spans="1:34" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>36</v>
@@ -5124,13 +5069,11 @@
       <c r="AG24" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH24" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH24" s="23"/>
     </row>
     <row r="25" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>36</v>
@@ -5144,17 +5087,17 @@
       <c r="E25" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F25" s="19" t="s">
-        <v>36</v>
+      <c r="F25" s="23" t="s">
+        <v>86</v>
       </c>
       <c r="G25" s="19" t="s">
         <v>36</v>
       </c>
       <c r="H25" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I25" s="54" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="J25" s="19" t="s">
         <v>36</v>
@@ -5166,7 +5109,7 @@
         <v>36</v>
       </c>
       <c r="M25" s="54" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="N25" s="19" t="s">
         <v>36</v>
@@ -5205,7 +5148,7 @@
         <v>36</v>
       </c>
       <c r="Z25" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AA25" s="19" t="s">
         <v>36</v>
@@ -5225,16 +5168,14 @@
       <c r="AF25" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG25" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH25" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AG25" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="AH25" s="23"/>
     </row>
     <row r="26" spans="1:34" s="51" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="52" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B26" s="23" t="s">
         <v>36</v>
@@ -5243,10 +5184,10 @@
         <v>36</v>
       </c>
       <c r="D26" s="54" t="s">
-        <v>146</v>
+        <v>85</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="F26" s="23" t="s">
         <v>36</v>
@@ -5258,7 +5199,7 @@
         <v>36</v>
       </c>
       <c r="I26" s="23" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="J26" s="23" t="s">
         <v>36</v>
@@ -5278,8 +5219,8 @@
       <c r="O26" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="P26" s="23" t="s">
-        <v>36</v>
+      <c r="P26" s="54" t="s">
+        <v>85</v>
       </c>
       <c r="Q26" s="23" t="s">
         <v>36</v>
@@ -5308,8 +5249,8 @@
       <c r="Y26" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="Z26" s="23" t="s">
-        <v>36</v>
+      <c r="Z26" s="54" t="s">
+        <v>40</v>
       </c>
       <c r="AA26" s="23" t="s">
         <v>36</v>
@@ -5332,117 +5273,47 @@
       <c r="AG26" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AH26" s="23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:34" s="51" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="52" t="s">
-        <v>142</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="C27" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="E27" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="F27" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="G27" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="H27" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="I27" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="J27" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="K27" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="L27" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="M27" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="N27" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="O27" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="P27" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q27" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="R27" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="S27" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="T27" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="U27" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="V27" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="W27" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="X27" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y27" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z27" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA27" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB27" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC27" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD27" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE27" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF27" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG27" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH27" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH26" s="23"/>
+    </row>
+    <row r="27" spans="1:34" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="52"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="23"/>
+      <c r="S27" s="23"/>
+      <c r="T27" s="23"/>
+      <c r="U27" s="23"/>
+      <c r="V27" s="23"/>
+      <c r="W27" s="23"/>
+      <c r="X27" s="23"/>
+      <c r="Y27" s="23"/>
+      <c r="Z27" s="23"/>
+      <c r="AA27" s="23"/>
+      <c r="AB27" s="23"/>
+      <c r="AC27" s="23"/>
+      <c r="AD27" s="23"/>
+      <c r="AE27" s="23"/>
+      <c r="AF27" s="23"/>
+      <c r="AG27" s="23"/>
+      <c r="AH27" s="23"/>
     </row>
     <row r="29" spans="1:34" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5469,18 +5340,18 @@
         <v>63</v>
       </c>
       <c r="I34" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="36" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
       <c r="B35" s="28" t="s">
         <v>86</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D35" s="46" t="s">
         <v>36</v>
@@ -5495,7 +5366,7 @@
         <v>98</v>
       </c>
       <c r="I35" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5515,7 +5386,7 @@
         <v>36</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G36" s="33" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
Пн 30.11.20 : 11:54:40,88
</commit_message>
<xml_diff>
--- a/eng.xlsx
+++ b/eng.xlsx
@@ -2597,8 +2597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B2:AG26"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35:G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5351,7 +5351,7 @@
         <v>86</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="D35" s="46" t="s">
         <v>36</v>

</xml_diff>